<commit_message>
switch from RunCACounties2 to RunCACounties
</commit_message>
<xml_diff>
--- a/Inputs/CAcounties.xlsx
+++ b/Inputs/CAcounties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB79250-12A1-044D-92DC-F61B91240609}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774482A2-42FC-F647-87AC-0B193FCF3C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="3900" windowWidth="29440" windowHeight="17100" activeTab="2" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
+    <workbookView xWindow="7820" yWindow="3820" windowWidth="29440" windowHeight="17100" activeTab="5" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -884,7 +884,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1015,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="4">
-        <v>0.36</v>
+        <v>0.18</v>
       </c>
       <c r="D9" s="4">
         <v>0.02</v>
@@ -1029,7 +1029,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="4">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="4">
         <v>0.05</v>
@@ -1058,7 +1058,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>43897</v>
+        <v>43905</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -1143,144 +1143,60 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>43907</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="3">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3">
-        <v>2</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>43920</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>7</v>
-      </c>
-      <c r="F6" s="3">
-        <v>2</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>43934</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E7" s="3">
-        <v>7</v>
-      </c>
-      <c r="F7" s="3">
-        <v>2</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>43948</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E8" s="3">
-        <v>7</v>
-      </c>
-      <c r="F8" s="3">
-        <v>2</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>43962</v>
-      </c>
-      <c r="B9" s="3">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E9" s="3">
-        <v>7</v>
-      </c>
-      <c r="F9" s="3">
-        <v>2</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>43976</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="3">
-        <v>7</v>
-      </c>
-      <c r="F10" s="3">
-        <v>2</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>43990</v>
-      </c>
-      <c r="B11" s="3">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="3">
-        <v>7</v>
-      </c>
-      <c r="F11" s="3">
-        <v>2</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1306,7 +1222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCB5455-61A0-9A48-A110-20902745EBF4}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -4897,7 +4813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DD5F9C-4676-5749-AB11-9739EC646DB2}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
scale uptake in counties
</commit_message>
<xml_diff>
--- a/Inputs/CAcounties.xlsx
+++ b/Inputs/CAcounties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1698B096-ABB2-8743-AC1B-287740A44F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E4BC61-26D9-594C-A940-79581D0CD023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30740" windowHeight="15040" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30740" windowHeight="15040" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -2564,7 +2564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2E9560-6072-47F8-9C1B-1CD23F686466}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2677,8 +2677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1D40A3-9166-4938-BDA5-A18F4C1841F8}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3112,7 +3112,7 @@
         <v>0.5</v>
       </c>
       <c r="M9" s="75">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="N9" s="75">
         <v>0.5</v>

</xml_diff>

<commit_message>
update for LEMMA v2.1
</commit_message>
<xml_diff>
--- a/Inputs/CAcounties.xlsx
+++ b/Inputs/CAcounties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF642F6-682F-6B42-AC24-84EEEAA91424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D63E96-FF61-2149-9AA3-A482FEE98FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30740" windowHeight="15040" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="5960" windowWidth="30740" windowHeight="15040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="166">
   <si>
     <t>Number of Days from Infection to Becoming Infectious (Latent Period)</t>
   </si>
@@ -520,6 +520,18 @@
   </si>
   <si>
     <t>epsilon</t>
+  </si>
+  <si>
+    <t>prior.infection.vaccine.scale</t>
+  </si>
+  <si>
+    <t>e.g. 0.8 = those with prior infection 20% less likely to get vaccinated than those without prior infection</t>
+  </si>
+  <si>
+    <t>child.transmission.scale</t>
+  </si>
+  <si>
+    <t>e.g. 0.7 = children age 0-11 are 30% less likely than adults to transmit if infected (due to biology and/or school mitigation)</t>
   </si>
 </sst>
 </file>
@@ -1416,7 +1428,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1544,14 +1556,27 @@
       </c>
     </row>
     <row r="11" spans="1:4" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="12" spans="1:4" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.5</v>
+      </c>
       <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
+      <c r="D12" s="52" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="13" spans="1:4" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
@@ -1589,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1676,20 +1701,44 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>44362</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>43831</formula1>
       <formula2>44196</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{0F9A4B89-EC6B-724F-B775-2FCA661AAF65}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B5" xr:uid="{0F9A4B89-EC6B-724F-B775-2FCA661AAF65}">
       <formula1>0</formula1>
       <formula2>30</formula2>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5" xr:uid="{5211C582-653B-1240-B539-BC7D547FCDE5}">
+      <formula1>43831</formula1>
+      <formula2>44561</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2075,7 +2124,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2250,7 +2299,7 @@
         <v>44166</v>
       </c>
       <c r="E11" s="58">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2266,7 +2315,7 @@
         <v>44166</v>
       </c>
       <c r="E12" s="58">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2565,7 +2614,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2611,10 +2660,10 @@
         <v>91</v>
       </c>
       <c r="C3" s="22">
-        <v>44317</v>
+        <v>44362</v>
       </c>
       <c r="D3" s="22">
-        <v>44317</v>
+        <v>44362</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2625,10 +2674,10 @@
         <v>94</v>
       </c>
       <c r="C4" s="19">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="D4" s="19">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2653,10 +2702,10 @@
         <v>80</v>
       </c>
       <c r="C6" s="19">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="D6" s="19">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2677,8 +2726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1D40A3-9166-4938-BDA5-A18F4C1841F8}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2829,10 +2878,10 @@
         <v>133</v>
       </c>
       <c r="B4" s="11">
-        <v>44221</v>
+        <v>44242</v>
       </c>
       <c r="C4" s="10">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="D4" s="57">
         <v>1</v>
@@ -2847,7 +2896,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="10">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="I4" s="58">
         <v>0.75</v>
@@ -2879,10 +2928,10 @@
         <v>157</v>
       </c>
       <c r="B5" s="11">
-        <v>44221</v>
+        <v>44362</v>
       </c>
       <c r="C5" s="10">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D5" s="10">
         <v>1.5</v>
@@ -2894,7 +2943,7 @@
         <v>1.5</v>
       </c>
       <c r="G5" s="10">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="H5" s="10">
         <v>1</v>
@@ -2929,10 +2978,10 @@
         <v>161</v>
       </c>
       <c r="B6" s="11">
-        <v>44221</v>
+        <v>44242</v>
       </c>
       <c r="C6" s="10">
-        <v>0.55000000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="D6" s="10">
         <v>1.25</v>
@@ -2947,7 +2996,7 @@
         <v>1.034</v>
       </c>
       <c r="H6" s="10">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="I6" s="58">
         <v>0.75</v>
@@ -2979,10 +3028,10 @@
         <v>160</v>
       </c>
       <c r="B7" s="11">
-        <v>44221</v>
+        <v>44362</v>
       </c>
       <c r="C7" s="10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D7" s="10">
         <v>1.8</v>
@@ -2994,7 +3043,7 @@
         <v>1.5</v>
       </c>
       <c r="G7" s="10">
-        <v>1</v>
+        <v>1.08</v>
       </c>
       <c r="H7" s="10">
         <v>1</v>
@@ -3029,7 +3078,7 @@
         <v>159</v>
       </c>
       <c r="B8" s="11">
-        <v>44221</v>
+        <v>44362</v>
       </c>
       <c r="C8" s="10">
         <v>0</v>
@@ -3044,7 +3093,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="10">
-        <v>1</v>
+        <v>1.04</v>
       </c>
       <c r="H8" s="10">
         <v>1</v>
@@ -3079,10 +3128,10 @@
         <v>158</v>
       </c>
       <c r="B9" s="11">
-        <v>44221</v>
+        <v>44362</v>
       </c>
       <c r="C9" s="10">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D9" s="74">
         <v>2.25</v>
@@ -3094,10 +3143,10 @@
         <v>1.5</v>
       </c>
       <c r="G9" s="74">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H9" s="74">
-        <v>1</v>
+        <v>1.08</v>
       </c>
       <c r="I9" s="75">
         <v>0.5</v>

</xml_diff>

<commit_message>
increase SD on June 15 change
</commit_message>
<xml_diff>
--- a/Inputs/CAcounties.xlsx
+++ b/Inputs/CAcounties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B7A7F0-E8A8-C349-85A8-3851A20BA672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C9E8E9-4F42-264F-BE18-7F736506DDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="5960" windowWidth="30740" windowHeight="15040" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="5960" windowWidth="30740" windowHeight="15040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -1616,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1712,7 +1712,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D5" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="3">
         <v>7</v>
@@ -2726,7 +2726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1D40A3-9166-4938-BDA5-A18F4C1841F8}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
increase base vaccine uptake
</commit_message>
<xml_diff>
--- a/Inputs/CAcounties.xlsx
+++ b/Inputs/CAcounties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE29846-22B2-7748-895B-8FA548484E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A378EF-7B87-6B43-8177-4B692F2FC5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="5960" windowWidth="30740" windowHeight="15040" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="5960" windowWidth="30740" windowHeight="15040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -2123,8 +2123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E08ED19-209C-1244-95CD-D0E05E30CCAF}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2179,7 +2179,7 @@
         <v>44562</v>
       </c>
       <c r="E3" s="58">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2194,7 +2194,7 @@
         <v>44562</v>
       </c>
       <c r="E4" s="58">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2209,7 +2209,7 @@
         <v>44329</v>
       </c>
       <c r="E5" s="58">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2224,7 +2224,7 @@
         <v>44166</v>
       </c>
       <c r="E6" s="58">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2239,7 +2239,7 @@
         <v>44166</v>
       </c>
       <c r="E7" s="58">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2254,7 +2254,7 @@
         <v>44166</v>
       </c>
       <c r="E8" s="58">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2269,7 +2269,7 @@
         <v>44166</v>
       </c>
       <c r="E9" s="58">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2299,7 +2299,7 @@
         <v>44166</v>
       </c>
       <c r="E11" s="58">
-        <v>0.85</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2315,7 +2315,7 @@
         <v>44166</v>
       </c>
       <c r="E12" s="58">
-        <v>0.85</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2613,7 +2613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2E9560-6072-47F8-9C1B-1CD23F686466}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>